<commit_message>
Template release for Optimus 2.0
</commit_message>
<xml_diff>
--- a/src/test/resources/elements/HelloOptimus.xlsx
+++ b/src/test/resources/elements/HelloOptimus.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>elementName</t>
   </si>
@@ -30,16 +30,19 @@
     <t>referTo</t>
   </si>
   <si>
-    <t>hola</t>
-  </si>
-  <si>
-    <t>aloh</t>
+    <t>WelcomeMessage</t>
   </si>
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>welcome_message</t>
+  </si>
+  <si>
     <t>presence</t>
+  </si>
+  <si>
+    <t>aloh</t>
   </si>
   <si>
     <t>abc</t>
@@ -1258,12 +1261,14 @@
       <c r="A2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" t="s" s="3">
+      <c r="B2" t="s" s="3">
         <v>6</v>
       </c>
+      <c r="C2" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="4"/>
@@ -1999,7 +2004,7 @@
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" t="s" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" t="s" s="3">
@@ -2740,13 +2745,13 @@
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="3">
-        <v>7</v>
-      </c>
       <c r="C2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s" s="3">
         <v>8</v>

</xml_diff>